<commit_message>
added most of the sensors we will probably want
3x temperature sensors
2x hall effect (for RPM)
2x battery voltage
1x current (inductive loop, 50A)
1x 3-axis gyro
1x 3-axis accelerometer
</commit_message>
<xml_diff>
--- a/parts.xlsx
+++ b/parts.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Part</t>
   </si>
@@ -48,9 +48,6 @@
     <t>SD card breakout</t>
   </si>
   <si>
-    <t>https://electropeak.com/micro-sd-tf-card-adapter-module</t>
-  </si>
-  <si>
     <t>https://lastminuteengineers.com/mpu6050-accel-gyro-arduino-tutorial/</t>
   </si>
   <si>
@@ -60,24 +57,70 @@
     <t>https://www.adafruit.com/product/372</t>
   </si>
   <si>
-    <t>cheaper and simpler than using a thermocouple module</t>
-  </si>
-  <si>
     <t>Quantity</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/adafruit-industries-llc/4682/12822319?WT.mc_id=frommaker.io</t>
+  </si>
+  <si>
+    <t>Hall effect sensor</t>
+  </si>
+  <si>
+    <t>https://maker.pro/arduino/tutorial/how-to-use-a-hall-effect-sensor-with-arduino#:~:text=The%20Arduino%20Hall%20effect%20sensor%20code%20can%20be%20used%20to,voltage%20to%20its%20Vout%20pin.</t>
+  </si>
+  <si>
+    <t>Can write directly from the SPI bus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cheaper and simpler than using a thermocouple </t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/melexis-technologies-nv/US5881LUA-AAA-000-BU/431876</t>
+  </si>
+  <si>
+    <t>Can use 1 on the motor or 2 for motor and axle</t>
+  </si>
+  <si>
+    <t>Current Sensor</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/lem-usa-inc/HAIS-50-P/1026520</t>
+  </si>
+  <si>
+    <t>Voltage Sensor IC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/analog-devices-inc/LTC2990CMS-TRPBF/2407346</t>
+  </si>
+  <si>
+    <t>4 channels, 2 for the battery and 2 for the ref and measurement on the current sensor</t>
+  </si>
+  <si>
+    <t>part cost</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -100,16 +143,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -388,19 +433,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.5703125" customWidth="1"/>
-    <col min="5" max="5" width="27.42578125" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -408,81 +453,175 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="1">
         <v>4</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D2" s="1">
+        <f>B2*C2</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>3.33</v>
       </c>
-      <c r="C3" s="3">
+      <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1">
+        <f t="shared" ref="D3:D8" si="0">B3*C3</f>
+        <v>3.33</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1</v>
+      </c>
+      <c r="C6" s="2">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="C6" s="3"/>
+      <c r="D6" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1">
+        <v>25.5</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
+        <v>25.5</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="1">
+        <v>6.7</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <f t="shared" si="0"/>
+        <v>6.7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" s="1">
+        <f>SUM(D2:D8)</f>
+        <v>56.53</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" display="https://www.amazon.com/HiLetgo-MPU-6050-Accelerometer-Gyroscope-Converter/dp/B00LP25V1A/ref=asc_df_B00LP25V1A/?tag=hyprod-20&amp;linkCode=df0&amp;hvadid=247487538123&amp;hvpos=&amp;hvnetw=g&amp;hvrand=10436269812826905526&amp;hvpone=&amp;hvptwo=&amp;hvqmt=&amp;hvdev=c&amp;hvdvcmdl=&amp;hvlocint=&amp;hv"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>